<commit_message>
🔄 Daily Excel update
</commit_message>
<xml_diff>
--- a/downloaded_file.xlsx
+++ b/downloaded_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://beltonene-my.sharepoint.com/personal/npacheco_beltonene_com/Documents/Pricing Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3151" documentId="8_{F3CD0FF8-58C3-41F7-B22B-5E277AA3B591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5FE7637-083B-4833-B7D8-E7B8C8DE19F1}"/>
+  <xr:revisionPtr revIDLastSave="3158" documentId="8_{F3CD0FF8-58C3-41F7-B22B-5E277AA3B591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27C4C5D4-A8D7-45A5-A583-DB49934DE360}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{117CC408-EBB5-49DC-AD42-2C9AA08047CD}"/>
+    <workbookView xWindow="1710" yWindow="1080" windowWidth="24525" windowHeight="15120" activeTab="1" xr2:uid="{117CC408-EBB5-49DC-AD42-2C9AA08047CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Calculator" sheetId="2" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2458" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2465" uniqueCount="600">
   <si>
     <t>Choose Hearing Aid model</t>
   </si>
@@ -2508,6 +2508,38 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2556,38 +2588,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3323,22 +3323,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0EDF487B-BC6A-43CC-A5E2-F07346E1A4ED}" name="HearingAids" displayName="HearingAids" ref="A1:P165" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
-  <autoFilter ref="A1:P165" xr:uid="{0EDF487B-BC6A-43CC-A5E2-F07346E1A4ED}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Beltone RIE Digital Envision 17 62S-DRWC"/>
-        <filter val="Beltone RIE Digital Envision 4 62S-DRWC"/>
-        <filter val="Beltone RIE Digital Envision 6 62S-DRWC"/>
-        <filter val="Beltone RIE Digital Envision 9 62S-DRWC"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Open House Special"/>
-        <filter val="Regular"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:P165" xr:uid="{0EDF487B-BC6A-43CC-A5E2-F07346E1A4ED}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P165">
     <sortCondition ref="E2:E165"/>
   </sortState>
@@ -3779,33 +3764,33 @@
   <sheetData>
     <row r="4" spans="1:20" ht="12" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:20" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="101" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="102"/>
+      <c r="B5" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="87"/>
       <c r="D5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="104" t="s">
+      <c r="E5" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="105"/>
+      <c r="F5" s="90"/>
       <c r="G5" s="82" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="84" t="s">
         <v>426</v>
       </c>
-      <c r="C6" s="100"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="25">
         <v>2</v>
       </c>
-      <c r="E6" s="106" t="s">
+      <c r="E6" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="107"/>
+      <c r="F6" s="92"/>
       <c r="G6" s="81" t="s">
         <v>598</v>
       </c>
@@ -3830,10 +3815,10 @@
       <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="103"/>
+      <c r="C10" s="88"/>
       <c r="E10" s="12" t="s">
         <v>452</v>
       </c>
@@ -3843,27 +3828,27 @@
       <c r="G10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="83" t="s">
+      <c r="J10" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="K10" s="83"/>
-      <c r="L10" s="83"/>
-      <c r="M10" s="83"/>
-      <c r="N10" s="83"/>
-      <c r="O10" s="83"/>
-      <c r="P10" s="83"/>
-      <c r="Q10" s="83"/>
+      <c r="K10" s="93"/>
+      <c r="L10" s="93"/>
+      <c r="M10" s="93"/>
+      <c r="N10" s="93"/>
+      <c r="O10" s="93"/>
+      <c r="P10" s="93"/>
+      <c r="Q10" s="93"/>
     </row>
     <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>446</v>
       </c>
-      <c r="B11" s="95" t="str">
+      <c r="B11" s="105" t="str">
         <f>IF($B$6="","",$B$6)</f>
         <v>Beltone RIE Digital Achieve 17 62DRWC</v>
       </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
       <c r="E11" s="50" cm="1">
         <f t="array" ref="E11">IF($B$6="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!F:F))</f>
         <v>5819</v>
@@ -3876,28 +3861,28 @@
         <f>E11-F11</f>
         <v>4300</v>
       </c>
-      <c r="J11" s="84" t="str" cm="1">
+      <c r="J11" s="94" t="str" cm="1">
         <f t="array" ref="J11">IF($B$6="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!D:D))</f>
         <v>(REG-HI-ACH17-62DRWC)</v>
       </c>
-      <c r="K11" s="85"/>
-      <c r="L11" s="85"/>
-      <c r="M11" s="85"/>
-      <c r="N11" s="85"/>
-      <c r="O11" s="85"/>
-      <c r="P11" s="85"/>
-      <c r="Q11" s="86"/>
+      <c r="K11" s="95"/>
+      <c r="L11" s="95"/>
+      <c r="M11" s="95"/>
+      <c r="N11" s="95"/>
+      <c r="O11" s="95"/>
+      <c r="P11" s="95"/>
+      <c r="Q11" s="96"/>
     </row>
     <row r="12" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>447</v>
       </c>
-      <c r="B12" s="95" t="str">
+      <c r="B12" s="105" t="str">
         <f>IF($D$6=1,"",B11)</f>
         <v>Beltone RIE Digital Achieve 17 62DRWC</v>
       </c>
-      <c r="C12" s="95"/>
-      <c r="D12" s="95"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
       <c r="E12" s="64" cm="1">
         <f t="array" ref="E12">IF($D$6=1,"0",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!F:F))</f>
         <v>5819</v>
@@ -3910,25 +3895,25 @@
         <f>E12-F12</f>
         <v>4300</v>
       </c>
-      <c r="J12" s="87"/>
-      <c r="K12" s="88"/>
-      <c r="L12" s="88"/>
-      <c r="M12" s="88"/>
-      <c r="N12" s="88"/>
-      <c r="O12" s="88"/>
-      <c r="P12" s="88"/>
-      <c r="Q12" s="89"/>
+      <c r="J12" s="97"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98"/>
+      <c r="O12" s="98"/>
+      <c r="P12" s="98"/>
+      <c r="Q12" s="99"/>
     </row>
     <row r="13" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="95" t="str" cm="1">
+      <c r="B13" s="105" t="str" cm="1">
         <f t="array" ref="B13">IF($B$6="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!G:G))</f>
         <v>Standard Charger</v>
       </c>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
       <c r="E13" s="13" cm="1">
         <f t="array" ref="E13">IF($B$13="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!H:H))</f>
         <v>250</v>
@@ -3941,26 +3926,26 @@
         <f t="array" ref="G13">IF($B$13="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!H:H))</f>
         <v>250</v>
       </c>
-      <c r="J13" s="87"/>
-      <c r="K13" s="88"/>
-      <c r="L13" s="88"/>
-      <c r="M13" s="88"/>
-      <c r="N13" s="88"/>
-      <c r="O13" s="88"/>
-      <c r="P13" s="88"/>
-      <c r="Q13" s="89"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="98"/>
+      <c r="P13" s="98"/>
+      <c r="Q13" s="99"/>
       <c r="T13" s="37"/>
     </row>
     <row r="14" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="95" t="str" cm="1">
+      <c r="B14" s="105" t="str" cm="1">
         <f t="array" ref="B14">IF($B$6="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!N:N))</f>
         <v>SureFit3 or M@RIE Receiver</v>
       </c>
-      <c r="C14" s="95"/>
-      <c r="D14" s="95"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="105"/>
       <c r="E14" s="48"/>
       <c r="F14" s="30" t="str" cm="1">
         <f t="array" ref="F14">IF($B$12="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!P:P))</f>
@@ -3970,26 +3955,26 @@
         <f t="array" ref="G14">IF($B$13="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!O:O/2))</f>
         <v>0</v>
       </c>
-      <c r="J14" s="87"/>
-      <c r="K14" s="88"/>
-      <c r="L14" s="88"/>
-      <c r="M14" s="88"/>
-      <c r="N14" s="88"/>
-      <c r="O14" s="88"/>
-      <c r="P14" s="88"/>
-      <c r="Q14" s="89"/>
+      <c r="J14" s="97"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="98"/>
+      <c r="M14" s="98"/>
+      <c r="N14" s="98"/>
+      <c r="O14" s="98"/>
+      <c r="P14" s="98"/>
+      <c r="Q14" s="99"/>
       <c r="T14" s="37"/>
     </row>
     <row r="15" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="95" t="str">
+      <c r="B15" s="105" t="str">
         <f>IF($D$6=1,"",B14)</f>
         <v>SureFit3 or M@RIE Receiver</v>
       </c>
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
       <c r="E15" s="48"/>
       <c r="F15" s="30" t="str" cm="1">
         <f t="array" ref="F15">IF($B$12="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!P:P))</f>
@@ -3999,46 +3984,46 @@
         <f t="array" ref="G15">IF($B$12="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!O:O/2))</f>
         <v>0</v>
       </c>
-      <c r="J15" s="87"/>
-      <c r="K15" s="88"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="88"/>
-      <c r="O15" s="88"/>
-      <c r="P15" s="88"/>
-      <c r="Q15" s="89"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98"/>
+      <c r="O15" s="98"/>
+      <c r="P15" s="98"/>
+      <c r="Q15" s="99"/>
     </row>
     <row r="16" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="91"/>
-      <c r="D16" s="91"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="101"/>
       <c r="E16" s="47"/>
       <c r="F16" s="47"/>
       <c r="G16" s="13">
         <f>SUM(G11:G15)</f>
         <v>8850</v>
       </c>
-      <c r="J16" s="92" t="str" cm="1">
+      <c r="J16" s="102" t="str" cm="1">
         <f t="array" ref="J16">IF($B$6="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!C:C))</f>
         <v>REG-HI-ACH17-62DRWC</v>
       </c>
-      <c r="K16" s="93"/>
-      <c r="L16" s="93"/>
-      <c r="M16" s="93"/>
-      <c r="N16" s="93"/>
-      <c r="O16" s="93"/>
-      <c r="P16" s="93"/>
-      <c r="Q16" s="94"/>
+      <c r="K16" s="103"/>
+      <c r="L16" s="103"/>
+      <c r="M16" s="103"/>
+      <c r="N16" s="103"/>
+      <c r="O16" s="103"/>
+      <c r="P16" s="103"/>
+      <c r="Q16" s="104"/>
     </row>
     <row r="17" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="91" t="str" cm="1">
+      <c r="B17" s="101" t="str" cm="1">
         <f t="array" ref="B17">IF($B$6="","",IF(_xlfn.XLOOKUP($B$6&amp;E6,haList!A:A&amp;haList!E:E,haList!M:M)=1,"PA Fitting Fee","(do not charge a PA Fitting Fee)"))</f>
         <v>PA Fitting Fee</v>
       </c>
-      <c r="C17" s="91"/>
-      <c r="D17" s="91"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="101"/>
       <c r="E17" s="47"/>
       <c r="F17" s="47"/>
       <c r="G17" s="13" cm="1">
@@ -4051,11 +4036,11 @@
       </c>
     </row>
     <row r="18" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="90" t="s">
+      <c r="B18" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="90"/>
-      <c r="D18" s="90"/>
+      <c r="C18" s="100"/>
+      <c r="D18" s="100"/>
       <c r="E18" s="49"/>
       <c r="F18" s="49"/>
       <c r="G18" s="14">
@@ -4065,9 +4050,9 @@
       <c r="I18" s="21"/>
     </row>
     <row r="19" spans="2:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="90"/>
-      <c r="C19" s="90"/>
-      <c r="D19" s="90"/>
+      <c r="B19" s="100"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="100"/>
       <c r="E19" s="49"/>
       <c r="F19" s="49"/>
       <c r="G19" s="14"/>
@@ -4079,12 +4064,12 @@
       <c r="G20" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="L20" s="84" t="e" cm="1" vm="1">
+      <c r="L20" s="94" t="e" cm="1" vm="1">
         <f t="array" aca="1" ref="L20" ca="1">_xlfn.IMAGE("https://chart.googleapis.com/chart?chs=500x500&amp;&amp;cht=qr&amp;chl="&amp;_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!C:C))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M20" s="85"/>
-      <c r="N20" s="86"/>
+      <c r="M20" s="95"/>
+      <c r="N20" s="96"/>
       <c r="O20" s="54"/>
       <c r="P20" s="54"/>
       <c r="Q20" s="54"/>
@@ -4098,9 +4083,9 @@
       <c r="G21" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="L21" s="87"/>
-      <c r="M21" s="88"/>
-      <c r="N21" s="89"/>
+      <c r="L21" s="97"/>
+      <c r="M21" s="98"/>
+      <c r="N21" s="99"/>
       <c r="O21" s="54"/>
       <c r="P21" s="54"/>
       <c r="Q21" s="54"/>
@@ -4118,9 +4103,9 @@
       <c r="H22" t="s">
         <v>453</v>
       </c>
-      <c r="L22" s="87"/>
-      <c r="M22" s="88"/>
-      <c r="N22" s="89"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="98"/>
+      <c r="N22" s="99"/>
       <c r="O22" s="54"/>
       <c r="P22" s="54"/>
       <c r="Q22" s="54"/>
@@ -4136,9 +4121,9 @@
       <c r="H23" t="s">
         <v>453</v>
       </c>
-      <c r="L23" s="87"/>
-      <c r="M23" s="88"/>
-      <c r="N23" s="89"/>
+      <c r="L23" s="97"/>
+      <c r="M23" s="98"/>
+      <c r="N23" s="99"/>
       <c r="O23" s="54"/>
       <c r="P23" s="54"/>
       <c r="Q23" s="54"/>
@@ -4157,9 +4142,9 @@
         <f>IF(E6="Anthem BCBS",((G16*60%)*G23)+G22,"")</f>
         <v/>
       </c>
-      <c r="L24" s="96"/>
-      <c r="M24" s="97"/>
-      <c r="N24" s="98"/>
+      <c r="L24" s="106"/>
+      <c r="M24" s="107"/>
+      <c r="N24" s="108"/>
       <c r="O24" s="54"/>
       <c r="P24" s="54"/>
       <c r="Q24" s="54"/>
@@ -4167,9 +4152,9 @@
       <c r="S24" s="54"/>
     </row>
     <row r="25" spans="2:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="90"/>
-      <c r="C25" s="90"/>
-      <c r="D25" s="90"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
       <c r="E25" s="49"/>
       <c r="F25" s="47" t="str">
         <f>IF($G$21='Data Lists'!C3,"Down Payment Type is Needed",IF($G$21='Data Lists'!C4,"20% down payment needed",IF($G$21='Data Lists'!C5,"20% down payment needed",IF($G$21='Data Lists'!C6,"$700 down payment needed",IF(AND($G$21='Data Lists'!C7,G18&gt;5555),"Down Payment Needed",IF(AND($G$21='Data Lists'!C7,G18&lt;5555),"10% Down Payment Needed"))))))</f>
@@ -4196,11 +4181,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="19">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
     <mergeCell ref="J10:Q10"/>
     <mergeCell ref="J11:Q15"/>
     <mergeCell ref="B25:D25"/>
@@ -4215,6 +4195,11 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="L20:N24"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6" xr:uid="{E095DD5D-12CC-4B09-A756-0B16300F1945}">
@@ -4258,10 +4243,10 @@
   <dimension ref="A1:Q314"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B147" sqref="B147"/>
+      <selection pane="bottomRight" activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -4336,7 +4321,7 @@
       </c>
       <c r="Q1"/>
     </row>
-    <row r="2" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="2" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A2" s="4" t="s">
         <v>454</v>
       </c>
@@ -4387,7 +4372,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="3" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A3" s="4" t="s">
         <v>455</v>
       </c>
@@ -4438,7 +4423,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="4" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A4" s="4" t="s">
         <v>456</v>
       </c>
@@ -4489,7 +4474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="5" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A5" s="71" t="s">
         <v>579</v>
       </c>
@@ -4537,11 +4522,13 @@
       </c>
       <c r="Q5"/>
     </row>
-    <row r="6" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="6" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A6" s="71" t="s">
         <v>575</v>
       </c>
-      <c r="B6" s="71"/>
+      <c r="B6" s="80" t="s">
+        <v>594</v>
+      </c>
       <c r="C6" s="4"/>
       <c r="D6" s="26" t="str">
         <f t="shared" si="0"/>
@@ -4584,11 +4571,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="7" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A7" s="71" t="s">
         <v>576</v>
       </c>
-      <c r="B7" s="71"/>
+      <c r="B7" s="80" t="s">
+        <v>595</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="26" t="str">
         <f t="shared" si="0"/>
@@ -4631,11 +4620,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="8" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A8" s="71" t="s">
         <v>577</v>
       </c>
-      <c r="B8" s="71"/>
+      <c r="B8" s="80" t="s">
+        <v>596</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="26" t="str">
         <f t="shared" si="0"/>
@@ -4678,7 +4669,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="9" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A9" s="4" t="s">
         <v>434</v>
       </c>
@@ -4725,7 +4716,7 @@
       </c>
       <c r="Q9"/>
     </row>
-    <row r="10" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="10" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A10" s="4" t="s">
         <v>435</v>
       </c>
@@ -4772,7 +4763,7 @@
       </c>
       <c r="Q10"/>
     </row>
-    <row r="11" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="11" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A11" s="4" t="s">
         <v>436</v>
       </c>
@@ -4819,7 +4810,7 @@
       </c>
       <c r="Q11"/>
     </row>
-    <row r="12" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="12" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A12" s="4" t="s">
         <v>59</v>
       </c>
@@ -4866,7 +4857,7 @@
       </c>
       <c r="Q12"/>
     </row>
-    <row r="13" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="13" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A13" s="4" t="s">
         <v>60</v>
       </c>
@@ -4913,7 +4904,7 @@
       </c>
       <c r="Q13"/>
     </row>
-    <row r="14" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="14" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A14" s="4" t="s">
         <v>61</v>
       </c>
@@ -4960,7 +4951,7 @@
       </c>
       <c r="Q14"/>
     </row>
-    <row r="15" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="15" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A15" s="4" t="s">
         <v>62</v>
       </c>
@@ -5007,7 +4998,7 @@
       </c>
       <c r="Q15"/>
     </row>
-    <row r="16" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="16" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A16" s="4" t="s">
         <v>63</v>
       </c>
@@ -5054,7 +5045,7 @@
       </c>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="17" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A17" s="4" t="s">
         <v>64</v>
       </c>
@@ -5101,7 +5092,7 @@
       </c>
       <c r="Q17"/>
     </row>
-    <row r="18" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="18" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -5152,7 +5143,7 @@
       </c>
       <c r="Q18"/>
     </row>
-    <row r="19" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="19" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A19" s="4" t="s">
         <v>52</v>
       </c>
@@ -5203,7 +5194,7 @@
       </c>
       <c r="Q19"/>
     </row>
-    <row r="20" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="20" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A20" s="4" t="s">
         <v>422</v>
       </c>
@@ -5254,7 +5245,7 @@
       </c>
       <c r="Q20"/>
     </row>
-    <row r="21" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="21" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -5305,7 +5296,7 @@
       </c>
       <c r="Q21"/>
     </row>
-    <row r="22" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="22" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
@@ -5351,7 +5342,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="23" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
@@ -5397,7 +5388,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="24" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A24" s="4" t="s">
         <v>39</v>
       </c>
@@ -5443,7 +5434,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="25" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A25" s="4" t="s">
         <v>40</v>
       </c>
@@ -5490,7 +5481,7 @@
       </c>
       <c r="Q25"/>
     </row>
-    <row r="26" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="26" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A26" s="4" t="s">
         <v>41</v>
       </c>
@@ -5537,7 +5528,7 @@
       </c>
       <c r="Q26"/>
     </row>
-    <row r="27" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="27" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A27" s="4" t="s">
         <v>42</v>
       </c>
@@ -5584,7 +5575,7 @@
       </c>
       <c r="Q27"/>
     </row>
-    <row r="28" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="28" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A28" s="4" t="s">
         <v>43</v>
       </c>
@@ -5631,7 +5622,7 @@
       </c>
       <c r="Q28"/>
     </row>
-    <row r="29" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="29" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A29" s="4" t="s">
         <v>44</v>
       </c>
@@ -5678,7 +5669,7 @@
       </c>
       <c r="Q29"/>
     </row>
-    <row r="30" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="30" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A30" s="4" t="s">
         <v>437</v>
       </c>
@@ -5725,7 +5716,7 @@
       </c>
       <c r="Q30"/>
     </row>
-    <row r="31" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="31" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A31" s="4" t="s">
         <v>443</v>
       </c>
@@ -5772,7 +5763,7 @@
       </c>
       <c r="Q31"/>
     </row>
-    <row r="32" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="32" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A32" s="4" t="s">
         <v>440</v>
       </c>
@@ -5819,7 +5810,7 @@
       </c>
       <c r="Q32"/>
     </row>
-    <row r="33" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="33" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A33" s="4" t="s">
         <v>23</v>
       </c>
@@ -5866,7 +5857,7 @@
       </c>
       <c r="Q33"/>
     </row>
-    <row r="34" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="34" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A34" s="4" t="s">
         <v>27</v>
       </c>
@@ -5913,7 +5904,7 @@
       </c>
       <c r="Q34"/>
     </row>
-    <row r="35" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="35" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A35" s="4" t="s">
         <v>438</v>
       </c>
@@ -5960,7 +5951,7 @@
       </c>
       <c r="Q35"/>
     </row>
-    <row r="36" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="36" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A36" s="4" t="s">
         <v>444</v>
       </c>
@@ -6007,7 +5998,7 @@
       </c>
       <c r="Q36"/>
     </row>
-    <row r="37" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="37" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A37" s="4" t="s">
         <v>441</v>
       </c>
@@ -6054,7 +6045,7 @@
       </c>
       <c r="Q37"/>
     </row>
-    <row r="38" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="38" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A38" s="4" t="s">
         <v>28</v>
       </c>
@@ -6101,7 +6092,7 @@
       </c>
       <c r="Q38"/>
     </row>
-    <row r="39" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="39" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A39" s="4" t="s">
         <v>29</v>
       </c>
@@ -6148,7 +6139,7 @@
       </c>
       <c r="Q39"/>
     </row>
-    <row r="40" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="40" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A40" s="4" t="s">
         <v>45</v>
       </c>
@@ -6193,7 +6184,7 @@
       <c r="P40" s="2"/>
       <c r="Q40"/>
     </row>
-    <row r="41" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="41" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A41" s="4" t="s">
         <v>439</v>
       </c>
@@ -6240,7 +6231,7 @@
       </c>
       <c r="Q41"/>
     </row>
-    <row r="42" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="42" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A42" s="4" t="s">
         <v>445</v>
       </c>
@@ -6287,7 +6278,7 @@
       </c>
       <c r="Q42"/>
     </row>
-    <row r="43" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="43" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A43" s="4" t="s">
         <v>442</v>
       </c>
@@ -6334,7 +6325,7 @@
       </c>
       <c r="Q43"/>
     </row>
-    <row r="44" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="44" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A44" s="4" t="s">
         <v>30</v>
       </c>
@@ -6379,7 +6370,7 @@
       <c r="P44" s="2"/>
       <c r="Q44"/>
     </row>
-    <row r="45" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="45" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A45" s="4" t="s">
         <v>46</v>
       </c>
@@ -6424,7 +6415,7 @@
       <c r="P45" s="2"/>
       <c r="Q45"/>
     </row>
-    <row r="46" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="46" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
@@ -6469,7 +6460,7 @@
       <c r="P46" s="2"/>
       <c r="Q46"/>
     </row>
-    <row r="47" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="47" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A47" s="4" t="s">
         <v>426</v>
       </c>
@@ -6520,7 +6511,7 @@
       </c>
       <c r="Q47"/>
     </row>
-    <row r="48" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="48" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A48" s="4" t="s">
         <v>428</v>
       </c>
@@ -6571,7 +6562,7 @@
       </c>
       <c r="Q48"/>
     </row>
-    <row r="49" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="49" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A49" s="4" t="s">
         <v>429</v>
       </c>
@@ -6622,7 +6613,7 @@
       </c>
       <c r="Q49"/>
     </row>
-    <row r="50" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="50" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A50" s="4" t="s">
         <v>31</v>
       </c>
@@ -6667,7 +6658,7 @@
       <c r="P50" s="2"/>
       <c r="Q50"/>
     </row>
-    <row r="51" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="51" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A51" s="4" t="s">
         <v>48</v>
       </c>
@@ -6712,7 +6703,7 @@
       <c r="P51" s="2"/>
       <c r="Q51"/>
     </row>
-    <row r="52" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="52" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A52" s="4" t="s">
         <v>49</v>
       </c>
@@ -6757,7 +6748,7 @@
       <c r="P52" s="2"/>
       <c r="Q52"/>
     </row>
-    <row r="53" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="53" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A53" s="4" t="s">
         <v>32</v>
       </c>
@@ -6802,7 +6793,7 @@
       <c r="P53" s="2"/>
       <c r="Q53"/>
     </row>
-    <row r="54" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="54" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A54" s="4" t="s">
         <v>51</v>
       </c>
@@ -6849,7 +6840,7 @@
       </c>
       <c r="Q54"/>
     </row>
-    <row r="55" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="55" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A55" s="4" t="s">
         <v>53</v>
       </c>
@@ -6896,7 +6887,7 @@
       </c>
       <c r="Q55"/>
     </row>
-    <row r="56" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="56" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A56" s="4" t="s">
         <v>35</v>
       </c>
@@ -6943,7 +6934,7 @@
       </c>
       <c r="Q56"/>
     </row>
-    <row r="57" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="57" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A57" s="4" t="s">
         <v>454</v>
       </c>
@@ -6993,7 +6984,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="58" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A58" s="4" t="s">
         <v>455</v>
       </c>
@@ -7043,7 +7034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="59" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A59" s="4" t="s">
         <v>456</v>
       </c>
@@ -7093,11 +7084,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="60" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A60" s="71" t="s">
         <v>575</v>
       </c>
-      <c r="B60" s="71"/>
+      <c r="B60" s="80" t="s">
+        <v>594</v>
+      </c>
       <c r="C60" s="71"/>
       <c r="D60" s="26" t="s">
         <v>582</v>
@@ -7139,11 +7132,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="61" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A61" s="71" t="s">
         <v>577</v>
       </c>
-      <c r="B61" s="71"/>
+      <c r="B61" s="80" t="s">
+        <v>595</v>
+      </c>
       <c r="C61" s="71"/>
       <c r="D61" s="26" t="s">
         <v>582</v>
@@ -7185,11 +7180,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="62" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A62" s="71" t="s">
         <v>576</v>
       </c>
-      <c r="B62" s="71"/>
+      <c r="B62" s="80" t="s">
+        <v>596</v>
+      </c>
       <c r="C62" s="71"/>
       <c r="D62" s="26" t="s">
         <v>582</v>
@@ -7231,11 +7228,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="63" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A63" s="71" t="s">
         <v>578</v>
       </c>
-      <c r="B63" s="71"/>
+      <c r="B63" s="83" t="s">
+        <v>599</v>
+      </c>
       <c r="C63" s="71"/>
       <c r="D63" s="26" t="s">
         <v>582</v>
@@ -7271,7 +7270,7 @@
       <c r="O63" s="77"/>
       <c r="P63" s="73"/>
     </row>
-    <row r="64" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="64" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A64" s="71" t="s">
         <v>579</v>
       </c>
@@ -7312,7 +7311,7 @@
       <c r="P64" s="73"/>
       <c r="Q64"/>
     </row>
-    <row r="65" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="65" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A65" s="71" t="s">
         <v>580</v>
       </c>
@@ -7353,7 +7352,7 @@
       <c r="P65" s="73"/>
       <c r="Q65"/>
     </row>
-    <row r="66" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="66" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A66" s="4" t="s">
         <v>454</v>
       </c>
@@ -7403,7 +7402,7 @@
       </c>
       <c r="Q66"/>
     </row>
-    <row r="67" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="67" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A67" s="4" t="s">
         <v>455</v>
       </c>
@@ -7453,7 +7452,7 @@
       </c>
       <c r="Q67"/>
     </row>
-    <row r="68" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="68" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A68" s="4" t="s">
         <v>456</v>
       </c>
@@ -7503,7 +7502,7 @@
       </c>
       <c r="Q68"/>
     </row>
-    <row r="69" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="69" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A69" s="71" t="s">
         <v>579</v>
       </c>
@@ -7551,7 +7550,7 @@
       </c>
       <c r="Q69"/>
     </row>
-    <row r="70" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="70" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A70" s="4" t="s">
         <v>454</v>
       </c>
@@ -7602,7 +7601,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="71" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A71" s="4" t="s">
         <v>455</v>
       </c>
@@ -7653,7 +7652,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="72" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A72" s="4" t="s">
         <v>456</v>
       </c>
@@ -7705,7 +7704,7 @@
       </c>
       <c r="Q72"/>
     </row>
-    <row r="73" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="73" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A73" s="71" t="s">
         <v>579</v>
       </c>
@@ -7757,7 +7756,7 @@
       </c>
       <c r="Q73"/>
     </row>
-    <row r="74" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="74" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A74" s="4" t="s">
         <v>454</v>
       </c>
@@ -7809,7 +7808,7 @@
       </c>
       <c r="Q74"/>
     </row>
-    <row r="75" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="75" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A75" s="4" t="s">
         <v>455</v>
       </c>
@@ -7861,7 +7860,7 @@
       </c>
       <c r="Q75"/>
     </row>
-    <row r="76" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="76" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A76" s="4" t="s">
         <v>456</v>
       </c>
@@ -7913,7 +7912,7 @@
       </c>
       <c r="Q76"/>
     </row>
-    <row r="77" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="77" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A77" s="71" t="s">
         <v>579</v>
       </c>
@@ -7965,7 +7964,7 @@
       </c>
       <c r="Q77"/>
     </row>
-    <row r="78" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="78" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A78" s="4" t="s">
         <v>454</v>
       </c>
@@ -8017,7 +8016,7 @@
       </c>
       <c r="Q78"/>
     </row>
-    <row r="79" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="79" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A79" s="4" t="s">
         <v>455</v>
       </c>
@@ -8069,7 +8068,7 @@
       </c>
       <c r="Q79"/>
     </row>
-    <row r="80" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="80" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A80" s="4" t="s">
         <v>456</v>
       </c>
@@ -8121,7 +8120,7 @@
       </c>
       <c r="Q80"/>
     </row>
-    <row r="81" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="81" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A81" s="71" t="s">
         <v>579</v>
       </c>
@@ -8173,7 +8172,7 @@
       </c>
       <c r="Q81"/>
     </row>
-    <row r="82" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="82" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A82" s="4" t="s">
         <v>454</v>
       </c>
@@ -8225,7 +8224,7 @@
       </c>
       <c r="Q82"/>
     </row>
-    <row r="83" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="83" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A83" s="4" t="s">
         <v>455</v>
       </c>
@@ -8277,7 +8276,7 @@
       </c>
       <c r="Q83"/>
     </row>
-    <row r="84" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="84" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A84" s="4" t="s">
         <v>456</v>
       </c>
@@ -8329,7 +8328,7 @@
       </c>
       <c r="Q84"/>
     </row>
-    <row r="85" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="85" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A85" s="71" t="s">
         <v>579</v>
       </c>
@@ -8381,7 +8380,7 @@
       </c>
       <c r="Q85"/>
     </row>
-    <row r="86" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="86" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A86" s="4" t="s">
         <v>454</v>
       </c>
@@ -8433,7 +8432,7 @@
       </c>
       <c r="Q86"/>
     </row>
-    <row r="87" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="87" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A87" s="4" t="s">
         <v>455</v>
       </c>
@@ -8485,7 +8484,7 @@
       </c>
       <c r="Q87" s="2"/>
     </row>
-    <row r="88" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="88" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A88" s="4" t="s">
         <v>456</v>
       </c>
@@ -8537,7 +8536,7 @@
       </c>
       <c r="Q88" s="2"/>
     </row>
-    <row r="89" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="89" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A89" s="71" t="s">
         <v>579</v>
       </c>
@@ -8739,7 +8738,7 @@
       </c>
       <c r="Q92" s="2"/>
     </row>
-    <row r="93" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="93" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A93" s="4" t="s">
         <v>434</v>
       </c>
@@ -8787,7 +8786,7 @@
       </c>
       <c r="Q93" s="2"/>
     </row>
-    <row r="94" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="94" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A94" s="4" t="s">
         <v>435</v>
       </c>
@@ -8835,7 +8834,7 @@
       </c>
       <c r="Q94" s="2"/>
     </row>
-    <row r="95" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="95" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A95" s="4" t="s">
         <v>436</v>
       </c>
@@ -8883,7 +8882,7 @@
       </c>
       <c r="Q95" s="2"/>
     </row>
-    <row r="96" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="96" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A96" s="4" t="s">
         <v>59</v>
       </c>
@@ -8931,7 +8930,7 @@
       </c>
       <c r="Q96" s="2"/>
     </row>
-    <row r="97" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="97" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A97" s="4" t="s">
         <v>60</v>
       </c>
@@ -8979,7 +8978,7 @@
       </c>
       <c r="Q97" s="2"/>
     </row>
-    <row r="98" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="98" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A98" s="4" t="s">
         <v>61</v>
       </c>
@@ -9027,7 +9026,7 @@
       </c>
       <c r="Q98" s="2"/>
     </row>
-    <row r="99" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="99" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A99" s="4" t="s">
         <v>62</v>
       </c>
@@ -9075,7 +9074,7 @@
       </c>
       <c r="Q99" s="2"/>
     </row>
-    <row r="100" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="100" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A100" s="4" t="s">
         <v>63</v>
       </c>
@@ -9123,7 +9122,7 @@
       </c>
       <c r="Q100" s="2"/>
     </row>
-    <row r="101" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="101" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A101" s="4" t="s">
         <v>64</v>
       </c>
@@ -9171,7 +9170,7 @@
       </c>
       <c r="Q101" s="2"/>
     </row>
-    <row r="102" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="102" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A102" s="4" t="s">
         <v>50</v>
       </c>
@@ -9223,7 +9222,7 @@
       </c>
       <c r="Q102" s="2"/>
     </row>
-    <row r="103" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="103" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A103" s="4" t="s">
         <v>52</v>
       </c>
@@ -9275,7 +9274,7 @@
       </c>
       <c r="Q103" s="2"/>
     </row>
-    <row r="104" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="104" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A104" s="4" t="s">
         <v>422</v>
       </c>
@@ -9327,7 +9326,7 @@
       </c>
       <c r="Q104" s="2"/>
     </row>
-    <row r="105" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="105" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A105" s="4" t="s">
         <v>33</v>
       </c>
@@ -9379,7 +9378,7 @@
       </c>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="106" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A106" s="4" t="s">
         <v>37</v>
       </c>
@@ -9427,7 +9426,7 @@
       </c>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="107" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A107" s="4" t="s">
         <v>38</v>
       </c>
@@ -9475,7 +9474,7 @@
       </c>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="108" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A108" s="4" t="s">
         <v>39</v>
       </c>
@@ -9523,7 +9522,7 @@
       </c>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="109" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A109" s="4" t="s">
         <v>40</v>
       </c>
@@ -9570,7 +9569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="110" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A110" s="4" t="s">
         <v>41</v>
       </c>
@@ -9617,7 +9616,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="111" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A111" s="4" t="s">
         <v>42</v>
       </c>
@@ -9664,7 +9663,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="112" spans="1:17" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A112" s="4" t="s">
         <v>43</v>
       </c>
@@ -9711,7 +9710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="113" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A113" s="4" t="s">
         <v>44</v>
       </c>
@@ -9758,7 +9757,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="114" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A114" s="4" t="s">
         <v>437</v>
       </c>
@@ -9805,7 +9804,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="115" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A115" s="4" t="s">
         <v>443</v>
       </c>
@@ -9852,7 +9851,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="116" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A116" s="4" t="s">
         <v>440</v>
       </c>
@@ -9899,7 +9898,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="117" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A117" s="4" t="s">
         <v>23</v>
       </c>
@@ -9946,7 +9945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="118" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A118" s="4" t="s">
         <v>27</v>
       </c>
@@ -9993,7 +9992,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="119" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A119" s="4" t="s">
         <v>438</v>
       </c>
@@ -10040,7 +10039,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="120" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A120" s="4" t="s">
         <v>444</v>
       </c>
@@ -10087,7 +10086,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="121" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A121" s="4" t="s">
         <v>441</v>
       </c>
@@ -10134,7 +10133,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="122" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A122" s="4" t="s">
         <v>28</v>
       </c>
@@ -10181,7 +10180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="123" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A123" s="4" t="s">
         <v>29</v>
       </c>
@@ -10228,7 +10227,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="124" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A124" s="4" t="s">
         <v>45</v>
       </c>
@@ -10273,7 +10272,7 @@
       </c>
       <c r="P124" s="2"/>
     </row>
-    <row r="125" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="125" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A125" s="4" t="s">
         <v>439</v>
       </c>
@@ -10320,7 +10319,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="126" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="126" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A126" s="4" t="s">
         <v>445</v>
       </c>
@@ -10367,7 +10366,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="127" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A127" s="4" t="s">
         <v>442</v>
       </c>
@@ -10414,7 +10413,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="128" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A128" s="4" t="s">
         <v>30</v>
       </c>
@@ -10459,7 +10458,7 @@
       </c>
       <c r="P128" s="2"/>
     </row>
-    <row r="129" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="129" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A129" s="4" t="s">
         <v>46</v>
       </c>
@@ -10504,7 +10503,7 @@
       </c>
       <c r="P129" s="2"/>
     </row>
-    <row r="130" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="130" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A130" s="4" t="s">
         <v>47</v>
       </c>
@@ -10549,7 +10548,7 @@
       </c>
       <c r="P130" s="2"/>
     </row>
-    <row r="131" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="131" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A131" s="4" t="s">
         <v>426</v>
       </c>
@@ -10600,7 +10599,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="132" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A132" s="4" t="s">
         <v>428</v>
       </c>
@@ -10651,7 +10650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="133" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A133" s="4" t="s">
         <v>429</v>
       </c>
@@ -10702,7 +10701,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="134" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A134" s="4" t="s">
         <v>31</v>
       </c>
@@ -10747,7 +10746,7 @@
       </c>
       <c r="P134" s="2"/>
     </row>
-    <row r="135" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="135" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A135" s="4" t="s">
         <v>48</v>
       </c>
@@ -10792,7 +10791,7 @@
       </c>
       <c r="P135" s="2"/>
     </row>
-    <row r="136" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="136" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A136" s="4" t="s">
         <v>49</v>
       </c>
@@ -10837,7 +10836,7 @@
       </c>
       <c r="P136" s="2"/>
     </row>
-    <row r="137" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="137" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A137" s="4" t="s">
         <v>32</v>
       </c>
@@ -10882,7 +10881,7 @@
       </c>
       <c r="P137" s="2"/>
     </row>
-    <row r="138" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="138" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A138" s="4" t="s">
         <v>51</v>
       </c>
@@ -10929,7 +10928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="139" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A139" s="4" t="s">
         <v>53</v>
       </c>
@@ -10976,7 +10975,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="140" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A140" s="4" t="s">
         <v>35</v>
       </c>
@@ -11023,7 +11022,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="141" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A141" s="4" t="s">
         <v>454</v>
       </c>
@@ -11074,7 +11073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="142" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A142" s="4" t="s">
         <v>455</v>
       </c>
@@ -11125,7 +11124,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="143" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A143" s="4" t="s">
         <v>456</v>
       </c>
@@ -11327,7 +11326,7 @@
       <c r="A147" s="71" t="s">
         <v>578</v>
       </c>
-      <c r="B147" s="108" t="s">
+      <c r="B147" s="83" t="s">
         <v>599</v>
       </c>
       <c r="C147" s="71"/>
@@ -11366,7 +11365,7 @@
       <c r="O147" s="77"/>
       <c r="P147" s="73"/>
     </row>
-    <row r="148" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="148" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A148" s="71" t="s">
         <v>579</v>
       </c>
@@ -11409,7 +11408,7 @@
       <c r="O148" s="77"/>
       <c r="P148" s="73"/>
     </row>
-    <row r="149" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="149" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A149" s="71" t="s">
         <v>580</v>
       </c>
@@ -11452,7 +11451,7 @@
       <c r="O149" s="77"/>
       <c r="P149" s="73"/>
     </row>
-    <row r="150" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="150" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A150" s="4" t="s">
         <v>454</v>
       </c>
@@ -11503,7 +11502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="151" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A151" s="4" t="s">
         <v>455</v>
       </c>
@@ -11554,7 +11553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="152" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A152" s="4" t="s">
         <v>456</v>
       </c>
@@ -11605,7 +11604,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="153" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="153" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A153" s="71" t="s">
         <v>579</v>
       </c>
@@ -11652,7 +11651,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="154" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="154" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A154" s="4" t="s">
         <v>454</v>
       </c>
@@ -11703,7 +11702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="155" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="155" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A155" s="4" t="s">
         <v>455</v>
       </c>
@@ -11754,7 +11753,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="156" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A156" s="4" t="s">
         <v>456</v>
       </c>
@@ -11805,7 +11804,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="157" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A157" s="71" t="s">
         <v>579</v>
       </c>
@@ -11852,7 +11851,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="158" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A158" s="4" t="s">
         <v>454</v>
       </c>
@@ -11903,7 +11902,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="159" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="159" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A159" s="4" t="s">
         <v>455</v>
       </c>
@@ -11954,7 +11953,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="160" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="160" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A160" s="4" t="s">
         <v>456</v>
       </c>
@@ -12005,7 +12004,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="161" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A161" s="71" t="s">
         <v>579</v>
       </c>
@@ -12052,7 +12051,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="162" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A162" s="4" t="s">
         <v>454</v>
       </c>
@@ -12103,7 +12102,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="163" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="163" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A163" s="4" t="s">
         <v>455</v>
       </c>
@@ -12154,7 +12153,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="164" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A164" s="4" t="s">
         <v>456</v>
       </c>
@@ -12205,7 +12204,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="165" spans="1:16" ht="24" hidden="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="165" spans="1:16" ht="24" x14ac:dyDescent="1.1499999999999999">
       <c r="A165" s="71" t="s">
         <v>579</v>
       </c>

</xml_diff>

<commit_message>
Fixed Commence 2 & 3 Listings
</commit_message>
<xml_diff>
--- a/downloaded_file.xlsx
+++ b/downloaded_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://beltonene-my.sharepoint.com/personal/npacheco_beltonene_com/Documents/Pricing Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3177" documentId="8_{F3CD0FF8-58C3-41F7-B22B-5E277AA3B591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9974DB61-F4A6-445B-9E69-B0AC11063800}"/>
+  <xr:revisionPtr revIDLastSave="3182" documentId="8_{F3CD0FF8-58C3-41F7-B22B-5E277AA3B591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{264C9757-7175-4634-BE14-4A73EB7E00B5}"/>
   <bookViews>
-    <workbookView xWindow="28500" yWindow="690" windowWidth="24525" windowHeight="15120" activeTab="1" xr2:uid="{117CC408-EBB5-49DC-AD42-2C9AA08047CD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{117CC408-EBB5-49DC-AD42-2C9AA08047CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Calculator" sheetId="2" r:id="rId1"/>
@@ -1880,10 +1880,10 @@
     <t>Beltone Envision 4 62S-DRWC Digital RIE</t>
   </si>
   <si>
-    <t>Beltone Commence 3 62S-DRWC Digital RIE</t>
-  </si>
-  <si>
-    <t>Beltone Commence 2 63S-DRWC Digital RIE</t>
+    <t>Beltone Commence 3 62-DRWC Digital RIE</t>
+  </si>
+  <si>
+    <t>Beltone Commence 2 63-DRW Digital RIE</t>
   </si>
 </sst>
 </file>
@@ -2369,7 +2369,7 @@
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2515,6 +2515,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2563,36 +2594,8 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3329,7 +3332,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0EDF487B-BC6A-43CC-A5E2-F07346E1A4ED}" name="HearingAids" displayName="HearingAids" ref="A1:P165" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
-  <autoFilter ref="A1:P165" xr:uid="{0EDF487B-BC6A-43CC-A5E2-F07346E1A4ED}"/>
+  <autoFilter ref="A1:P165" xr:uid="{0EDF487B-BC6A-43CC-A5E2-F07346E1A4ED}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Beltone Commence 2 63S-DRWC Digital RIE"/>
+        <filter val="Beltone Commence 3 62S-DRWC Digital RIE"/>
+        <filter val="Beltone Envision 17 62S-DRWC Digital RIE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P165">
     <sortCondition ref="E2:E165"/>
   </sortState>
@@ -3761,33 +3772,33 @@
   <sheetData>
     <row r="4" spans="1:20" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="103"/>
+      <c r="B5" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="87"/>
       <c r="D5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="105" t="s">
+      <c r="E5" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="106"/>
+      <c r="F5" s="90"/>
       <c r="G5" s="82" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="100" t="s">
+      <c r="B6" s="84" t="s">
         <v>426</v>
       </c>
-      <c r="C6" s="101"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="25">
         <v>2</v>
       </c>
-      <c r="E6" s="107" t="s">
+      <c r="E6" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="108"/>
+      <c r="F6" s="92"/>
       <c r="G6" s="81" t="s">
         <v>598</v>
       </c>
@@ -3812,10 +3823,10 @@
       <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="104" t="s">
+      <c r="B10" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="104"/>
+      <c r="C10" s="88"/>
       <c r="E10" s="12" t="s">
         <v>452</v>
       </c>
@@ -3825,27 +3836,27 @@
       <c r="G10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="84" t="s">
+      <c r="J10" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="K10" s="84"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="84"/>
-      <c r="N10" s="84"/>
-      <c r="O10" s="84"/>
-      <c r="P10" s="84"/>
-      <c r="Q10" s="84"/>
+      <c r="K10" s="93"/>
+      <c r="L10" s="93"/>
+      <c r="M10" s="93"/>
+      <c r="N10" s="93"/>
+      <c r="O10" s="93"/>
+      <c r="P10" s="93"/>
+      <c r="Q10" s="93"/>
     </row>
     <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>446</v>
       </c>
-      <c r="B11" s="96" t="str">
+      <c r="B11" s="105" t="str">
         <f>IF($B$6="","",$B$6)</f>
         <v>Beltone RIE Digital Achieve 17 62DRWC</v>
       </c>
-      <c r="C11" s="96"/>
-      <c r="D11" s="96"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
       <c r="E11" s="50" cm="1">
         <f t="array" ref="E11">IF($B$6="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!F:F))</f>
         <v>5819</v>
@@ -3858,28 +3869,28 @@
         <f>E11-F11</f>
         <v>4300</v>
       </c>
-      <c r="J11" s="85" t="str" cm="1">
+      <c r="J11" s="94" t="str" cm="1">
         <f t="array" ref="J11">IF($B$6="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!D:D))</f>
         <v>(REG-HI-ACH17-62DRWC)</v>
       </c>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
-      <c r="N11" s="86"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="86"/>
-      <c r="Q11" s="87"/>
+      <c r="K11" s="95"/>
+      <c r="L11" s="95"/>
+      <c r="M11" s="95"/>
+      <c r="N11" s="95"/>
+      <c r="O11" s="95"/>
+      <c r="P11" s="95"/>
+      <c r="Q11" s="96"/>
     </row>
     <row r="12" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>447</v>
       </c>
-      <c r="B12" s="96" t="str">
+      <c r="B12" s="105" t="str">
         <f>IF($D$6=1,"",B11)</f>
         <v>Beltone RIE Digital Achieve 17 62DRWC</v>
       </c>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
       <c r="E12" s="64" cm="1">
         <f t="array" ref="E12">IF($D$6=1,"0",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!F:F))</f>
         <v>5819</v>
@@ -3892,25 +3903,25 @@
         <f>E12-F12</f>
         <v>4300</v>
       </c>
-      <c r="J12" s="88"/>
-      <c r="K12" s="89"/>
-      <c r="L12" s="89"/>
-      <c r="M12" s="89"/>
-      <c r="N12" s="89"/>
-      <c r="O12" s="89"/>
-      <c r="P12" s="89"/>
-      <c r="Q12" s="90"/>
+      <c r="J12" s="97"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98"/>
+      <c r="O12" s="98"/>
+      <c r="P12" s="98"/>
+      <c r="Q12" s="99"/>
     </row>
     <row r="13" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="96" t="str" cm="1">
+      <c r="B13" s="105" t="str" cm="1">
         <f t="array" ref="B13">IF($B$6="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!G:G))</f>
         <v>Standard Charger</v>
       </c>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
       <c r="E13" s="13" cm="1">
         <f t="array" ref="E13">IF($B$13="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!H:H))</f>
         <v>250</v>
@@ -3923,26 +3934,26 @@
         <f t="array" ref="G13">IF($B$13="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!H:H))</f>
         <v>250</v>
       </c>
-      <c r="J13" s="88"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="89"/>
-      <c r="N13" s="89"/>
-      <c r="O13" s="89"/>
-      <c r="P13" s="89"/>
-      <c r="Q13" s="90"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="98"/>
+      <c r="P13" s="98"/>
+      <c r="Q13" s="99"/>
       <c r="T13" s="37"/>
     </row>
     <row r="14" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="96" t="str" cm="1">
+      <c r="B14" s="105" t="str" cm="1">
         <f t="array" ref="B14">IF($B$6="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!N:N))</f>
         <v>SureFit3 or M@RIE Receiver</v>
       </c>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="105"/>
       <c r="E14" s="48"/>
       <c r="F14" s="30" t="str" cm="1">
         <f t="array" ref="F14">IF($B$12="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!P:P))</f>
@@ -3952,26 +3963,26 @@
         <f t="array" ref="G14">IF($B$13="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!O:O/2))</f>
         <v>0</v>
       </c>
-      <c r="J14" s="88"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="89"/>
-      <c r="M14" s="89"/>
-      <c r="N14" s="89"/>
-      <c r="O14" s="89"/>
-      <c r="P14" s="89"/>
-      <c r="Q14" s="90"/>
+      <c r="J14" s="97"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="98"/>
+      <c r="M14" s="98"/>
+      <c r="N14" s="98"/>
+      <c r="O14" s="98"/>
+      <c r="P14" s="98"/>
+      <c r="Q14" s="99"/>
       <c r="T14" s="37"/>
     </row>
     <row r="15" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="96" t="str">
+      <c r="B15" s="105" t="str">
         <f>IF($D$6=1,"",B14)</f>
         <v>SureFit3 or M@RIE Receiver</v>
       </c>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
       <c r="E15" s="48"/>
       <c r="F15" s="30" t="str" cm="1">
         <f t="array" ref="F15">IF($B$12="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!P:P))</f>
@@ -3981,46 +3992,46 @@
         <f t="array" ref="G15">IF($B$12="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!O:O/2))</f>
         <v>0</v>
       </c>
-      <c r="J15" s="88"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="89"/>
-      <c r="M15" s="89"/>
-      <c r="N15" s="89"/>
-      <c r="O15" s="89"/>
-      <c r="P15" s="89"/>
-      <c r="Q15" s="90"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98"/>
+      <c r="O15" s="98"/>
+      <c r="P15" s="98"/>
+      <c r="Q15" s="99"/>
     </row>
     <row r="16" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="101"/>
       <c r="E16" s="47"/>
       <c r="F16" s="47"/>
       <c r="G16" s="13">
         <f>SUM(G11:G15)</f>
         <v>8850</v>
       </c>
-      <c r="J16" s="93" t="str" cm="1">
+      <c r="J16" s="102" t="str" cm="1">
         <f t="array" ref="J16">IF($B$6="","",_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!C:C))</f>
         <v>REG-HI-ACH17-62DRWC</v>
       </c>
-      <c r="K16" s="94"/>
-      <c r="L16" s="94"/>
-      <c r="M16" s="94"/>
-      <c r="N16" s="94"/>
-      <c r="O16" s="94"/>
-      <c r="P16" s="94"/>
-      <c r="Q16" s="95"/>
+      <c r="K16" s="103"/>
+      <c r="L16" s="103"/>
+      <c r="M16" s="103"/>
+      <c r="N16" s="103"/>
+      <c r="O16" s="103"/>
+      <c r="P16" s="103"/>
+      <c r="Q16" s="104"/>
     </row>
     <row r="17" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="92" t="str" cm="1">
+      <c r="B17" s="101" t="str" cm="1">
         <f t="array" ref="B17">IF($B$6="","",IF(_xlfn.XLOOKUP($B$6&amp;E6,haList!A:A&amp;haList!E:E,haList!M:M)=1,"PA Fitting Fee","(do not charge a PA Fitting Fee)"))</f>
         <v>PA Fitting Fee</v>
       </c>
-      <c r="C17" s="92"/>
-      <c r="D17" s="92"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="101"/>
       <c r="E17" s="47"/>
       <c r="F17" s="47"/>
       <c r="G17" s="13" cm="1">
@@ -4033,11 +4044,11 @@
       </c>
     </row>
     <row r="18" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="91"/>
-      <c r="D18" s="91"/>
+      <c r="C18" s="100"/>
+      <c r="D18" s="100"/>
       <c r="E18" s="49"/>
       <c r="F18" s="49"/>
       <c r="G18" s="14">
@@ -4047,9 +4058,9 @@
       <c r="I18" s="21"/>
     </row>
     <row r="19" spans="2:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
+      <c r="B19" s="100"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="100"/>
       <c r="E19" s="49"/>
       <c r="F19" s="49"/>
       <c r="G19" s="14"/>
@@ -4061,12 +4072,12 @@
       <c r="G20" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="L20" s="85" t="e" cm="1" vm="1">
+      <c r="L20" s="94" t="e" cm="1" vm="1">
         <f t="array" aca="1" ref="L20" ca="1">_xlfn.IMAGE("https://chart.googleapis.com/chart?chs=500x500&amp;&amp;cht=qr&amp;chl="&amp;_xlfn.XLOOKUP($B$6&amp;$E$6,haList!A:A&amp;haList!E:E,haList!C:C))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M20" s="86"/>
-      <c r="N20" s="87"/>
+      <c r="M20" s="95"/>
+      <c r="N20" s="96"/>
       <c r="O20" s="54"/>
       <c r="P20" s="54"/>
       <c r="Q20" s="54"/>
@@ -4080,9 +4091,9 @@
       <c r="G21" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="L21" s="88"/>
-      <c r="M21" s="89"/>
-      <c r="N21" s="90"/>
+      <c r="L21" s="97"/>
+      <c r="M21" s="98"/>
+      <c r="N21" s="99"/>
       <c r="O21" s="54"/>
       <c r="P21" s="54"/>
       <c r="Q21" s="54"/>
@@ -4100,9 +4111,9 @@
       <c r="H22" t="s">
         <v>453</v>
       </c>
-      <c r="L22" s="88"/>
-      <c r="M22" s="89"/>
-      <c r="N22" s="90"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="98"/>
+      <c r="N22" s="99"/>
       <c r="O22" s="54"/>
       <c r="P22" s="54"/>
       <c r="Q22" s="54"/>
@@ -4118,9 +4129,9 @@
       <c r="H23" t="s">
         <v>453</v>
       </c>
-      <c r="L23" s="88"/>
-      <c r="M23" s="89"/>
-      <c r="N23" s="90"/>
+      <c r="L23" s="97"/>
+      <c r="M23" s="98"/>
+      <c r="N23" s="99"/>
       <c r="O23" s="54"/>
       <c r="P23" s="54"/>
       <c r="Q23" s="54"/>
@@ -4139,9 +4150,9 @@
         <f>IF(E6="Anthem BCBS",((G16*60%)*G23)+G22,"")</f>
         <v/>
       </c>
-      <c r="L24" s="97"/>
-      <c r="M24" s="98"/>
-      <c r="N24" s="99"/>
+      <c r="L24" s="106"/>
+      <c r="M24" s="107"/>
+      <c r="N24" s="108"/>
       <c r="O24" s="54"/>
       <c r="P24" s="54"/>
       <c r="Q24" s="54"/>
@@ -4149,9 +4160,9 @@
       <c r="S24" s="54"/>
     </row>
     <row r="25" spans="2:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="91"/>
-      <c r="C25" s="91"/>
-      <c r="D25" s="91"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
       <c r="E25" s="49"/>
       <c r="F25" s="47" t="str">
         <f>IF($G$21='Data Lists'!C3,"Down Payment Type is Needed",IF($G$21='Data Lists'!C4,"20% down payment needed",IF($G$21='Data Lists'!C5,"20% down payment needed",IF($G$21='Data Lists'!C6,"$700 down payment needed",IF(AND($G$21='Data Lists'!C7,G18&gt;5555),"Down Payment Needed",IF(AND($G$21='Data Lists'!C7,G18&lt;5555),"10% Down Payment Needed"))))))</f>
@@ -4178,11 +4189,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="19">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
     <mergeCell ref="J10:Q10"/>
     <mergeCell ref="J11:Q15"/>
     <mergeCell ref="B25:D25"/>
@@ -4197,6 +4203,11 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="L20:N24"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6" xr:uid="{E095DD5D-12CC-4B09-A756-0B16300F1945}">
@@ -4240,10 +4251,10 @@
   <dimension ref="A1:Q314"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B137" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B148" sqref="B148"/>
+      <selection pane="bottomRight" activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -4318,7 +4329,7 @@
       </c>
       <c r="Q1"/>
     </row>
-    <row r="2" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A2" s="4" t="s">
         <v>454</v>
       </c>
@@ -4369,7 +4380,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A3" s="4" t="s">
         <v>455</v>
       </c>
@@ -4420,7 +4431,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A4" s="4" t="s">
         <v>456</v>
       </c>
@@ -4471,7 +4482,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A5" s="71" t="s">
         <v>579</v>
       </c>
@@ -4568,7 +4579,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A7" s="71" t="s">
         <v>576</v>
       </c>
@@ -4617,7 +4628,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A8" s="71" t="s">
         <v>577</v>
       </c>
@@ -4666,7 +4677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A9" s="4" t="s">
         <v>434</v>
       </c>
@@ -4713,7 +4724,7 @@
       </c>
       <c r="Q9"/>
     </row>
-    <row r="10" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A10" s="4" t="s">
         <v>435</v>
       </c>
@@ -4760,7 +4771,7 @@
       </c>
       <c r="Q10"/>
     </row>
-    <row r="11" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A11" s="4" t="s">
         <v>436</v>
       </c>
@@ -4807,7 +4818,7 @@
       </c>
       <c r="Q11"/>
     </row>
-    <row r="12" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="12" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A12" s="4" t="s">
         <v>59</v>
       </c>
@@ -4854,7 +4865,7 @@
       </c>
       <c r="Q12"/>
     </row>
-    <row r="13" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A13" s="4" t="s">
         <v>60</v>
       </c>
@@ -4901,7 +4912,7 @@
       </c>
       <c r="Q13"/>
     </row>
-    <row r="14" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A14" s="4" t="s">
         <v>61</v>
       </c>
@@ -4948,7 +4959,7 @@
       </c>
       <c r="Q14"/>
     </row>
-    <row r="15" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A15" s="4" t="s">
         <v>62</v>
       </c>
@@ -4995,7 +5006,7 @@
       </c>
       <c r="Q15"/>
     </row>
-    <row r="16" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="16" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A16" s="4" t="s">
         <v>63</v>
       </c>
@@ -5042,7 +5053,7 @@
       </c>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="17" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A17" s="4" t="s">
         <v>64</v>
       </c>
@@ -5089,7 +5100,7 @@
       </c>
       <c r="Q17"/>
     </row>
-    <row r="18" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="18" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -5140,7 +5151,7 @@
       </c>
       <c r="Q18"/>
     </row>
-    <row r="19" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A19" s="4" t="s">
         <v>52</v>
       </c>
@@ -5191,7 +5202,7 @@
       </c>
       <c r="Q19"/>
     </row>
-    <row r="20" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A20" s="4" t="s">
         <v>422</v>
       </c>
@@ -5242,7 +5253,7 @@
       </c>
       <c r="Q20"/>
     </row>
-    <row r="21" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="21" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -5293,7 +5304,7 @@
       </c>
       <c r="Q21"/>
     </row>
-    <row r="22" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
@@ -5339,7 +5350,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="23" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
@@ -5385,7 +5396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="24" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A24" s="4" t="s">
         <v>39</v>
       </c>
@@ -5431,7 +5442,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="25" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A25" s="4" t="s">
         <v>40</v>
       </c>
@@ -5478,7 +5489,7 @@
       </c>
       <c r="Q25"/>
     </row>
-    <row r="26" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="26" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A26" s="4" t="s">
         <v>41</v>
       </c>
@@ -5525,7 +5536,7 @@
       </c>
       <c r="Q26"/>
     </row>
-    <row r="27" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="27" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A27" s="4" t="s">
         <v>42</v>
       </c>
@@ -5572,7 +5583,7 @@
       </c>
       <c r="Q27"/>
     </row>
-    <row r="28" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="28" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A28" s="4" t="s">
         <v>43</v>
       </c>
@@ -5619,7 +5630,7 @@
       </c>
       <c r="Q28"/>
     </row>
-    <row r="29" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="29" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A29" s="4" t="s">
         <v>44</v>
       </c>
@@ -5666,7 +5677,7 @@
       </c>
       <c r="Q29"/>
     </row>
-    <row r="30" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="30" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A30" s="4" t="s">
         <v>437</v>
       </c>
@@ -5713,7 +5724,7 @@
       </c>
       <c r="Q30"/>
     </row>
-    <row r="31" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="31" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A31" s="4" t="s">
         <v>443</v>
       </c>
@@ -5760,7 +5771,7 @@
       </c>
       <c r="Q31"/>
     </row>
-    <row r="32" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="32" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A32" s="4" t="s">
         <v>440</v>
       </c>
@@ -5807,7 +5818,7 @@
       </c>
       <c r="Q32"/>
     </row>
-    <row r="33" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="33" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A33" s="4" t="s">
         <v>23</v>
       </c>
@@ -5854,7 +5865,7 @@
       </c>
       <c r="Q33"/>
     </row>
-    <row r="34" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="34" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A34" s="4" t="s">
         <v>27</v>
       </c>
@@ -5901,7 +5912,7 @@
       </c>
       <c r="Q34"/>
     </row>
-    <row r="35" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="35" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A35" s="4" t="s">
         <v>438</v>
       </c>
@@ -5948,7 +5959,7 @@
       </c>
       <c r="Q35"/>
     </row>
-    <row r="36" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="36" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A36" s="4" t="s">
         <v>444</v>
       </c>
@@ -5995,7 +6006,7 @@
       </c>
       <c r="Q36"/>
     </row>
-    <row r="37" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="37" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A37" s="4" t="s">
         <v>441</v>
       </c>
@@ -6042,7 +6053,7 @@
       </c>
       <c r="Q37"/>
     </row>
-    <row r="38" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="38" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A38" s="4" t="s">
         <v>28</v>
       </c>
@@ -6089,7 +6100,7 @@
       </c>
       <c r="Q38"/>
     </row>
-    <row r="39" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="39" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A39" s="4" t="s">
         <v>29</v>
       </c>
@@ -6136,7 +6147,7 @@
       </c>
       <c r="Q39"/>
     </row>
-    <row r="40" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="40" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A40" s="4" t="s">
         <v>45</v>
       </c>
@@ -6181,7 +6192,7 @@
       <c r="P40" s="2"/>
       <c r="Q40"/>
     </row>
-    <row r="41" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="41" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A41" s="4" t="s">
         <v>439</v>
       </c>
@@ -6228,7 +6239,7 @@
       </c>
       <c r="Q41"/>
     </row>
-    <row r="42" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="42" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A42" s="4" t="s">
         <v>445</v>
       </c>
@@ -6275,7 +6286,7 @@
       </c>
       <c r="Q42"/>
     </row>
-    <row r="43" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="43" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A43" s="4" t="s">
         <v>442</v>
       </c>
@@ -6322,7 +6333,7 @@
       </c>
       <c r="Q43"/>
     </row>
-    <row r="44" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="44" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A44" s="4" t="s">
         <v>30</v>
       </c>
@@ -6367,7 +6378,7 @@
       <c r="P44" s="2"/>
       <c r="Q44"/>
     </row>
-    <row r="45" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="45" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A45" s="4" t="s">
         <v>46</v>
       </c>
@@ -6412,7 +6423,7 @@
       <c r="P45" s="2"/>
       <c r="Q45"/>
     </row>
-    <row r="46" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="46" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
@@ -6457,7 +6468,7 @@
       <c r="P46" s="2"/>
       <c r="Q46"/>
     </row>
-    <row r="47" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="47" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A47" s="4" t="s">
         <v>426</v>
       </c>
@@ -6508,7 +6519,7 @@
       </c>
       <c r="Q47"/>
     </row>
-    <row r="48" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="48" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A48" s="4" t="s">
         <v>428</v>
       </c>
@@ -6559,7 +6570,7 @@
       </c>
       <c r="Q48"/>
     </row>
-    <row r="49" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="49" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A49" s="4" t="s">
         <v>429</v>
       </c>
@@ -6610,7 +6621,7 @@
       </c>
       <c r="Q49"/>
     </row>
-    <row r="50" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="50" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A50" s="4" t="s">
         <v>31</v>
       </c>
@@ -6655,7 +6666,7 @@
       <c r="P50" s="2"/>
       <c r="Q50"/>
     </row>
-    <row r="51" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="51" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A51" s="4" t="s">
         <v>48</v>
       </c>
@@ -6700,7 +6711,7 @@
       <c r="P51" s="2"/>
       <c r="Q51"/>
     </row>
-    <row r="52" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="52" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A52" s="4" t="s">
         <v>49</v>
       </c>
@@ -6745,7 +6756,7 @@
       <c r="P52" s="2"/>
       <c r="Q52"/>
     </row>
-    <row r="53" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="53" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A53" s="4" t="s">
         <v>32</v>
       </c>
@@ -6790,7 +6801,7 @@
       <c r="P53" s="2"/>
       <c r="Q53"/>
     </row>
-    <row r="54" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="54" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A54" s="4" t="s">
         <v>51</v>
       </c>
@@ -6837,7 +6848,7 @@
       </c>
       <c r="Q54"/>
     </row>
-    <row r="55" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="55" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A55" s="4" t="s">
         <v>53</v>
       </c>
@@ -6884,7 +6895,7 @@
       </c>
       <c r="Q55"/>
     </row>
-    <row r="56" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="56" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A56" s="4" t="s">
         <v>35</v>
       </c>
@@ -6931,7 +6942,7 @@
       </c>
       <c r="Q56"/>
     </row>
-    <row r="57" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="57" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A57" s="4" t="s">
         <v>454</v>
       </c>
@@ -6981,7 +6992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="58" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A58" s="4" t="s">
         <v>455</v>
       </c>
@@ -7031,7 +7042,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="59" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A59" s="4" t="s">
         <v>456</v>
       </c>
@@ -7129,7 +7140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="61" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A61" s="71" t="s">
         <v>577</v>
       </c>
@@ -7177,7 +7188,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="62" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A62" s="71" t="s">
         <v>576</v>
       </c>
@@ -7225,7 +7236,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="63" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A63" s="71" t="s">
         <v>578</v>
       </c>
@@ -7267,7 +7278,7 @@
       <c r="O63" s="77"/>
       <c r="P63" s="73"/>
     </row>
-    <row r="64" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="64" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A64" s="71" t="s">
         <v>579</v>
       </c>
@@ -7308,7 +7319,7 @@
       <c r="P64" s="73"/>
       <c r="Q64"/>
     </row>
-    <row r="65" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="65" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A65" s="71" t="s">
         <v>580</v>
       </c>
@@ -7349,7 +7360,7 @@
       <c r="P65" s="73"/>
       <c r="Q65"/>
     </row>
-    <row r="66" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="66" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A66" s="4" t="s">
         <v>454</v>
       </c>
@@ -7399,7 +7410,7 @@
       </c>
       <c r="Q66"/>
     </row>
-    <row r="67" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="67" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A67" s="4" t="s">
         <v>455</v>
       </c>
@@ -7449,7 +7460,7 @@
       </c>
       <c r="Q67"/>
     </row>
-    <row r="68" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="68" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A68" s="4" t="s">
         <v>456</v>
       </c>
@@ -7499,7 +7510,7 @@
       </c>
       <c r="Q68"/>
     </row>
-    <row r="69" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="69" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A69" s="71" t="s">
         <v>579</v>
       </c>
@@ -7547,7 +7558,7 @@
       </c>
       <c r="Q69"/>
     </row>
-    <row r="70" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="70" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A70" s="4" t="s">
         <v>454</v>
       </c>
@@ -7598,7 +7609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="71" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A71" s="4" t="s">
         <v>455</v>
       </c>
@@ -7649,7 +7660,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="72" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A72" s="4" t="s">
         <v>456</v>
       </c>
@@ -7701,7 +7712,7 @@
       </c>
       <c r="Q72"/>
     </row>
-    <row r="73" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="73" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A73" s="71" t="s">
         <v>579</v>
       </c>
@@ -7753,7 +7764,7 @@
       </c>
       <c r="Q73"/>
     </row>
-    <row r="74" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="74" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A74" s="4" t="s">
         <v>454</v>
       </c>
@@ -7805,7 +7816,7 @@
       </c>
       <c r="Q74"/>
     </row>
-    <row r="75" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="75" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A75" s="4" t="s">
         <v>455</v>
       </c>
@@ -7857,7 +7868,7 @@
       </c>
       <c r="Q75"/>
     </row>
-    <row r="76" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="76" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A76" s="4" t="s">
         <v>456</v>
       </c>
@@ -7909,7 +7920,7 @@
       </c>
       <c r="Q76"/>
     </row>
-    <row r="77" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="77" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A77" s="71" t="s">
         <v>579</v>
       </c>
@@ -7961,7 +7972,7 @@
       </c>
       <c r="Q77"/>
     </row>
-    <row r="78" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="78" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A78" s="4" t="s">
         <v>454</v>
       </c>
@@ -8013,7 +8024,7 @@
       </c>
       <c r="Q78"/>
     </row>
-    <row r="79" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="79" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A79" s="4" t="s">
         <v>455</v>
       </c>
@@ -8065,7 +8076,7 @@
       </c>
       <c r="Q79"/>
     </row>
-    <row r="80" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="80" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A80" s="4" t="s">
         <v>456</v>
       </c>
@@ -8117,7 +8128,7 @@
       </c>
       <c r="Q80"/>
     </row>
-    <row r="81" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="81" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A81" s="71" t="s">
         <v>579</v>
       </c>
@@ -8169,7 +8180,7 @@
       </c>
       <c r="Q81"/>
     </row>
-    <row r="82" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="82" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A82" s="4" t="s">
         <v>454</v>
       </c>
@@ -8221,7 +8232,7 @@
       </c>
       <c r="Q82"/>
     </row>
-    <row r="83" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="83" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A83" s="4" t="s">
         <v>455</v>
       </c>
@@ -8273,7 +8284,7 @@
       </c>
       <c r="Q83"/>
     </row>
-    <row r="84" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="84" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A84" s="4" t="s">
         <v>456</v>
       </c>
@@ -8325,7 +8336,7 @@
       </c>
       <c r="Q84"/>
     </row>
-    <row r="85" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="85" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A85" s="71" t="s">
         <v>579</v>
       </c>
@@ -8377,7 +8388,7 @@
       </c>
       <c r="Q85"/>
     </row>
-    <row r="86" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="86" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A86" s="4" t="s">
         <v>454</v>
       </c>
@@ -8429,7 +8440,7 @@
       </c>
       <c r="Q86"/>
     </row>
-    <row r="87" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="87" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A87" s="4" t="s">
         <v>455</v>
       </c>
@@ -8481,7 +8492,7 @@
       </c>
       <c r="Q87" s="2"/>
     </row>
-    <row r="88" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="88" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A88" s="4" t="s">
         <v>456</v>
       </c>
@@ -8533,7 +8544,7 @@
       </c>
       <c r="Q88" s="2"/>
     </row>
-    <row r="89" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="89" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A89" s="71" t="s">
         <v>579</v>
       </c>
@@ -8635,7 +8646,7 @@
       </c>
       <c r="Q90" s="2"/>
     </row>
-    <row r="91" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="91" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A91" s="71" t="s">
         <v>576</v>
       </c>
@@ -8685,7 +8696,7 @@
       </c>
       <c r="Q91" s="2"/>
     </row>
-    <row r="92" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="92" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A92" s="71" t="s">
         <v>577</v>
       </c>
@@ -8735,7 +8746,7 @@
       </c>
       <c r="Q92" s="2"/>
     </row>
-    <row r="93" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="93" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A93" s="4" t="s">
         <v>434</v>
       </c>
@@ -8783,7 +8794,7 @@
       </c>
       <c r="Q93" s="2"/>
     </row>
-    <row r="94" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="94" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A94" s="4" t="s">
         <v>435</v>
       </c>
@@ -8831,7 +8842,7 @@
       </c>
       <c r="Q94" s="2"/>
     </row>
-    <row r="95" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="95" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A95" s="4" t="s">
         <v>436</v>
       </c>
@@ -8879,7 +8890,7 @@
       </c>
       <c r="Q95" s="2"/>
     </row>
-    <row r="96" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="96" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A96" s="4" t="s">
         <v>59</v>
       </c>
@@ -8927,7 +8938,7 @@
       </c>
       <c r="Q96" s="2"/>
     </row>
-    <row r="97" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="97" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A97" s="4" t="s">
         <v>60</v>
       </c>
@@ -8975,7 +8986,7 @@
       </c>
       <c r="Q97" s="2"/>
     </row>
-    <row r="98" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="98" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A98" s="4" t="s">
         <v>61</v>
       </c>
@@ -9023,7 +9034,7 @@
       </c>
       <c r="Q98" s="2"/>
     </row>
-    <row r="99" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="99" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A99" s="4" t="s">
         <v>62</v>
       </c>
@@ -9071,7 +9082,7 @@
       </c>
       <c r="Q99" s="2"/>
     </row>
-    <row r="100" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="100" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A100" s="4" t="s">
         <v>63</v>
       </c>
@@ -9119,7 +9130,7 @@
       </c>
       <c r="Q100" s="2"/>
     </row>
-    <row r="101" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="101" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A101" s="4" t="s">
         <v>64</v>
       </c>
@@ -9167,7 +9178,7 @@
       </c>
       <c r="Q101" s="2"/>
     </row>
-    <row r="102" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="102" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A102" s="4" t="s">
         <v>50</v>
       </c>
@@ -9219,7 +9230,7 @@
       </c>
       <c r="Q102" s="2"/>
     </row>
-    <row r="103" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="103" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A103" s="4" t="s">
         <v>52</v>
       </c>
@@ -9271,7 +9282,7 @@
       </c>
       <c r="Q103" s="2"/>
     </row>
-    <row r="104" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="104" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A104" s="4" t="s">
         <v>422</v>
       </c>
@@ -9323,7 +9334,7 @@
       </c>
       <c r="Q104" s="2"/>
     </row>
-    <row r="105" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="105" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A105" s="4" t="s">
         <v>33</v>
       </c>
@@ -9375,7 +9386,7 @@
       </c>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="106" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A106" s="4" t="s">
         <v>37</v>
       </c>
@@ -9423,7 +9434,7 @@
       </c>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="107" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A107" s="4" t="s">
         <v>38</v>
       </c>
@@ -9471,7 +9482,7 @@
       </c>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="108" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A108" s="4" t="s">
         <v>39</v>
       </c>
@@ -9519,7 +9530,7 @@
       </c>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="109" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A109" s="4" t="s">
         <v>40</v>
       </c>
@@ -9566,7 +9577,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="110" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A110" s="4" t="s">
         <v>41</v>
       </c>
@@ -9613,7 +9624,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="111" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A111" s="4" t="s">
         <v>42</v>
       </c>
@@ -9660,7 +9671,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="112" spans="1:17" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A112" s="4" t="s">
         <v>43</v>
       </c>
@@ -9707,7 +9718,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="113" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A113" s="4" t="s">
         <v>44</v>
       </c>
@@ -9754,7 +9765,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="114" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A114" s="4" t="s">
         <v>437</v>
       </c>
@@ -9801,7 +9812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="115" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A115" s="4" t="s">
         <v>443</v>
       </c>
@@ -9848,7 +9859,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="116" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A116" s="4" t="s">
         <v>440</v>
       </c>
@@ -9895,7 +9906,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="117" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A117" s="4" t="s">
         <v>23</v>
       </c>
@@ -9942,7 +9953,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="118" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A118" s="4" t="s">
         <v>27</v>
       </c>
@@ -9989,7 +10000,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="119" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A119" s="4" t="s">
         <v>438</v>
       </c>
@@ -10036,7 +10047,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="120" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A120" s="4" t="s">
         <v>444</v>
       </c>
@@ -10083,7 +10094,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="121" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A121" s="4" t="s">
         <v>441</v>
       </c>
@@ -10130,7 +10141,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="122" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A122" s="4" t="s">
         <v>28</v>
       </c>
@@ -10177,7 +10188,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="123" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A123" s="4" t="s">
         <v>29</v>
       </c>
@@ -10224,7 +10235,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="124" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A124" s="4" t="s">
         <v>45</v>
       </c>
@@ -10269,7 +10280,7 @@
       </c>
       <c r="P124" s="2"/>
     </row>
-    <row r="125" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="125" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A125" s="4" t="s">
         <v>439</v>
       </c>
@@ -10316,7 +10327,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="126" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="126" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A126" s="4" t="s">
         <v>445</v>
       </c>
@@ -10363,7 +10374,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="127" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A127" s="4" t="s">
         <v>442</v>
       </c>
@@ -10410,7 +10421,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="128" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A128" s="4" t="s">
         <v>30</v>
       </c>
@@ -10455,7 +10466,7 @@
       </c>
       <c r="P128" s="2"/>
     </row>
-    <row r="129" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="129" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A129" s="4" t="s">
         <v>46</v>
       </c>
@@ -10500,7 +10511,7 @@
       </c>
       <c r="P129" s="2"/>
     </row>
-    <row r="130" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="130" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A130" s="4" t="s">
         <v>47</v>
       </c>
@@ -10545,7 +10556,7 @@
       </c>
       <c r="P130" s="2"/>
     </row>
-    <row r="131" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="131" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A131" s="4" t="s">
         <v>426</v>
       </c>
@@ -10596,7 +10607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="132" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A132" s="4" t="s">
         <v>428</v>
       </c>
@@ -10647,7 +10658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="133" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A133" s="4" t="s">
         <v>429</v>
       </c>
@@ -10698,7 +10709,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="134" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A134" s="4" t="s">
         <v>31</v>
       </c>
@@ -10743,7 +10754,7 @@
       </c>
       <c r="P134" s="2"/>
     </row>
-    <row r="135" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="135" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A135" s="4" t="s">
         <v>48</v>
       </c>
@@ -10788,7 +10799,7 @@
       </c>
       <c r="P135" s="2"/>
     </row>
-    <row r="136" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="136" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A136" s="4" t="s">
         <v>49</v>
       </c>
@@ -10833,7 +10844,7 @@
       </c>
       <c r="P136" s="2"/>
     </row>
-    <row r="137" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="137" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A137" s="4" t="s">
         <v>32</v>
       </c>
@@ -10878,7 +10889,7 @@
       </c>
       <c r="P137" s="2"/>
     </row>
-    <row r="138" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="138" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A138" s="4" t="s">
         <v>51</v>
       </c>
@@ -10925,7 +10936,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="139" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A139" s="4" t="s">
         <v>53</v>
       </c>
@@ -10972,7 +10983,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="140" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A140" s="4" t="s">
         <v>35</v>
       </c>
@@ -11019,7 +11030,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="141" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A141" s="4" t="s">
         <v>454</v>
       </c>
@@ -11070,7 +11081,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="142" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A142" s="4" t="s">
         <v>455</v>
       </c>
@@ -11121,7 +11132,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="143" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A143" s="4" t="s">
         <v>456</v>
       </c>
@@ -11184,7 +11195,7 @@
         <f t="shared" si="8"/>
         <v>()</v>
       </c>
-      <c r="E144" s="72" t="s">
+      <c r="E144" s="109" t="s">
         <v>2</v>
       </c>
       <c r="F144" s="73">
@@ -11221,7 +11232,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="145" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A145" s="71" t="s">
         <v>577</v>
       </c>
@@ -11270,7 +11281,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="146" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A146" s="71" t="s">
         <v>576</v>
       </c>
@@ -11319,7 +11330,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="147" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A147" s="71" t="s">
         <v>578</v>
       </c>
@@ -11448,7 +11459,7 @@
       <c r="O149" s="77"/>
       <c r="P149" s="73"/>
     </row>
-    <row r="150" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="150" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A150" s="4" t="s">
         <v>454</v>
       </c>
@@ -11499,7 +11510,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="151" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A151" s="4" t="s">
         <v>455</v>
       </c>
@@ -11550,7 +11561,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="152" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A152" s="4" t="s">
         <v>456</v>
       </c>
@@ -11601,7 +11612,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="153" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="153" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A153" s="71" t="s">
         <v>579</v>
       </c>
@@ -11648,7 +11659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="154" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="154" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A154" s="4" t="s">
         <v>454</v>
       </c>
@@ -11699,7 +11710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="155" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="155" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A155" s="4" t="s">
         <v>455</v>
       </c>
@@ -11750,7 +11761,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="156" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A156" s="4" t="s">
         <v>456</v>
       </c>
@@ -11801,7 +11812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="157" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A157" s="71" t="s">
         <v>579</v>
       </c>
@@ -11848,7 +11859,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="158" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A158" s="4" t="s">
         <v>454</v>
       </c>
@@ -11899,7 +11910,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="159" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="159" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A159" s="4" t="s">
         <v>455</v>
       </c>
@@ -11950,7 +11961,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="160" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="160" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A160" s="4" t="s">
         <v>456</v>
       </c>
@@ -12001,7 +12012,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="161" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A161" s="71" t="s">
         <v>579</v>
       </c>
@@ -12048,7 +12059,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="162" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A162" s="4" t="s">
         <v>454</v>
       </c>
@@ -12099,7 +12110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="163" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="163" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A163" s="4" t="s">
         <v>455</v>
       </c>
@@ -12150,7 +12161,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="164" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A164" s="4" t="s">
         <v>456</v>
       </c>
@@ -12201,7 +12212,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="165" spans="1:16" ht="21.75" x14ac:dyDescent="0.7">
+    <row r="165" spans="1:16" ht="21.75" hidden="1" x14ac:dyDescent="0.7">
       <c r="A165" s="71" t="s">
         <v>579</v>
       </c>

</xml_diff>